<commit_message>
Implemented #9: Support summary autofill.
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -4,28 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Do not scan 1" sheetId="1" r:id="rId1"/>
     <sheet name="Do not scan 2" sheetId="2" r:id="rId2"/>
     <sheet name="# Scan 1" sheetId="3" r:id="rId3"/>
     <sheet name="# Scan 2" sheetId="4" r:id="rId4"/>
-    <sheet name="!!! Forbidden issues" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>IssueDescription</t>
-  </si>
-  <si>
     <t>IssueKey</t>
   </si>
   <si>
@@ -209,25 +205,13 @@
     <t>PRJ-22</t>
   </si>
   <si>
-    <t>Root issues</t>
-  </si>
-  <si>
-    <t>Task #0</t>
-  </si>
-  <si>
-    <t>PRJ-0</t>
-  </si>
-  <si>
-    <t>Task #99</t>
-  </si>
-  <si>
-    <t>PRJ-99</t>
-  </si>
-  <si>
-    <t>1. Find differences</t>
-  </si>
-  <si>
-    <t>2. Copy values from new to old and save</t>
+    <t>IssueSummary</t>
+  </si>
+  <si>
+    <t>Press Ctrl+Alt+Shift+F9 to recalculate all formulas!</t>
+  </si>
+  <si>
+    <t>Copy values from "New values" to "Old values" with date to see changes next time.</t>
   </si>
 </sst>
 </file>
@@ -261,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,18 +267,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,6 +433,58 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -488,96 +512,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -961,9 +907,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A16:P32"/>
+  <dimension ref="A15:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P17" sqref="P17:P18"/>
     </sheetView>
   </sheetViews>
@@ -986,113 +932,132 @@
     <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+    </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="D17" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="32" t="s">
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="45"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="38" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40" t="s">
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="23"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="46"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>15</v>
+      <c r="A20" s="41" t="s">
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="4">
         <v>8</v>
@@ -1104,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="4">
         <v>8</v>
@@ -1116,7 +1081,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L20" s="5">
         <f>H20-D20</f>
@@ -1136,12 +1101,12 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="4">
         <v>7</v>
@@ -1153,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="4">
         <v>7</v>
@@ -1165,7 +1130,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" ref="L21:L25" si="1">H21-D21</f>
@@ -1185,12 +1150,12 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="4">
         <v>8</v>
@@ -1202,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
@@ -1214,7 +1179,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="1"/>
@@ -1234,12 +1199,12 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="4">
         <v>9</v>
@@ -1251,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="4">
         <v>5</v>
@@ -1263,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="1"/>
@@ -1283,12 +1248,12 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="4">
         <v>7</v>
@@ -1300,7 +1265,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="4">
         <v>7</v>
@@ -1312,7 +1277,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="1"/>
@@ -1332,12 +1297,12 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25" s="4">
         <v>8</v>
@@ -1349,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="4">
         <v>8</v>
@@ -1361,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="1"/>
@@ -1381,12 +1346,12 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="D26" s="8">
         <f>SUM(D20:D25)</f>
@@ -1438,14 +1403,14 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>16</v>
+      <c r="A27" s="41" t="s">
+        <v>15</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="12">
         <v>16</v>
@@ -1457,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H27" s="12">
         <v>16</v>
@@ -1469,7 +1434,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L27" s="12">
         <f t="shared" si="5"/>
@@ -1489,12 +1454,12 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D28" s="4">
         <v>15</v>
@@ -1506,7 +1471,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="4">
         <v>14</v>
@@ -1518,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" ref="L28:L31" si="7">H28-D28</f>
@@ -1538,12 +1503,12 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D29" s="4">
         <v>14</v>
@@ -1555,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="4">
         <v>13</v>
@@ -1567,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="7"/>
@@ -1587,12 +1552,12 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D30" s="4">
         <v>13</v>
@@ -1604,7 +1569,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="4">
         <v>13</v>
@@ -1616,7 +1581,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="7"/>
@@ -1636,12 +1601,12 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D31" s="4">
         <v>12</v>
@@ -1653,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -1665,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L31" s="21">
         <f t="shared" si="7"/>
@@ -1685,12 +1650,12 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="D32" s="8">
         <f>SUM(D27:D31)</f>
@@ -1742,30 +1707,32 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:K17"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:K17"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:O32 L20:O25">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:O26">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:O31">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1776,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A16:P32"/>
+  <dimension ref="A15:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:P18"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,114 +1768,133 @@
     <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+    </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="D17" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="32" t="s">
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="23"/>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="45"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="38" t="s">
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="40" t="s">
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="23"/>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="46"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P19" s="51"/>
+      <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>15</v>
+      <c r="A20" s="41" t="s">
+        <v>14</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="4">
         <v>9</v>
@@ -1920,7 +1906,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="4">
         <v>8</v>
@@ -1932,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L20" s="5">
         <f>H20-D20</f>
@@ -1952,12 +1938,12 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="4">
         <v>8</v>
@@ -1969,7 +1955,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="4">
         <v>7</v>
@@ -1981,7 +1967,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" ref="L21:M32" si="1">H21-D21</f>
@@ -2001,12 +1987,12 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="4">
         <v>9</v>
@@ -2018,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
@@ -2030,7 +2016,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="1"/>
@@ -2050,12 +2036,12 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="4">
         <v>10</v>
@@ -2067,7 +2053,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="4">
         <v>5</v>
@@ -2079,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="1"/>
@@ -2099,12 +2085,12 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" s="4">
         <v>8</v>
@@ -2116,7 +2102,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="4">
         <v>7</v>
@@ -2128,7 +2114,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="1"/>
@@ -2148,12 +2134,12 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="4">
         <v>9</v>
@@ -2165,7 +2151,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="4">
         <v>8</v>
@@ -2177,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L25" s="5">
         <f t="shared" si="1"/>
@@ -2197,12 +2183,12 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
+      <c r="A26" s="43"/>
       <c r="B26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="D26" s="8">
         <f>SUM(D20:D25)</f>
@@ -2254,14 +2240,14 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
-        <v>16</v>
+      <c r="A27" s="41" t="s">
+        <v>15</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" s="12">
         <v>17</v>
@@ -2273,7 +2259,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H27" s="12">
         <v>16</v>
@@ -2285,7 +2271,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L27" s="12">
         <f t="shared" si="1"/>
@@ -2305,12 +2291,12 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" s="4">
         <v>16</v>
@@ -2322,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="4">
         <v>14</v>
@@ -2334,7 +2320,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="1"/>
@@ -2354,12 +2340,12 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" s="4">
         <v>15</v>
@@ -2371,7 +2357,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="4">
         <v>13</v>
@@ -2383,7 +2369,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="1"/>
@@ -2403,12 +2389,12 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="4">
         <v>14</v>
@@ -2420,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="4">
         <v>13</v>
@@ -2432,7 +2418,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="1"/>
@@ -2452,12 +2438,12 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="24"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31" s="4">
         <v>13</v>
@@ -2469,7 +2455,7 @@
         <v>4</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -2481,7 +2467,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L31" s="21">
         <f t="shared" si="1"/>
@@ -2501,12 +2487,12 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
+      <c r="A32" s="43"/>
       <c r="B32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>14</v>
       </c>
       <c r="D32" s="8">
         <f>SUM(D27:D31)</f>
@@ -2558,331 +2544,36 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="H17:K17"/>
     <mergeCell ref="L17:O18"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="H18:K18"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:O32 L20:O25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:O26">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27:O31">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="51" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="4">
-        <v>8</v>
-      </c>
-      <c r="E4" s="5">
-        <v>8</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L4" s="5">
-        <f>H4-D4</f>
-        <v>-8</v>
-      </c>
-      <c r="M4" s="5">
-        <f t="shared" ref="M4:N6" si="0">I4-E4</f>
-        <v>-8</v>
-      </c>
-      <c r="N4" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <f>IF(G4=K4,0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="5">
-        <f>H5-D5</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" ref="M5" si="1">I5-E5</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" ref="N5" si="2">J5-F5</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
-        <f>IF(G5=K5,0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="8">
-        <f>SUM(D4:D4)</f>
-        <v>8</v>
-      </c>
-      <c r="E6" s="9">
-        <f>SUM(E4:E4)</f>
-        <v>8</v>
-      </c>
-      <c r="F6" s="9">
-        <f>SUM(F4:F4)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="8">
-        <f>SUM(H4:H4)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
-        <f>SUM(I4:I4)</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="9">
-        <f>SUM(J4:J4)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="9">
-        <f t="shared" ref="L6" si="3">H6-D6</f>
-        <v>-8</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="0"/>
-        <v>-8</v>
-      </c>
-      <c r="N6" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="L4:O5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L6:O6">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented #11: Process all cells until the end of document.
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="21075" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19965" windowHeight="13020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Do not scan 1" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,12 @@
     <sheet name="# Scan 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <oleSize ref="A1:S41"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -56,9 +57,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>skip</t>
   </si>
   <si>
     <t>Task pile #1</t>
@@ -434,6 +432,39 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -484,39 +515,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -909,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A15:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:P18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,85 +931,85 @@
   </cols>
   <sheetData>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-    </row>
-    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="38" t="s">
+      <c r="A17" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="24" t="s">
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="37"/>
       <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="30" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32" t="s">
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="29"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="40"/>
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1050,14 +1048,14 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
-        <v>14</v>
+      <c r="A20" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4">
         <v>8</v>
@@ -1101,12 +1099,12 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="4">
         <v>7</v>
@@ -1118,7 +1116,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="4">
         <v>7</v>
@@ -1130,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" ref="L21:L25" si="1">H21-D21</f>
@@ -1150,12 +1148,12 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4">
         <v>8</v>
@@ -1167,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
@@ -1179,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="1"/>
@@ -1199,12 +1197,12 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="4">
         <v>9</v>
@@ -1216,7 +1214,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="4">
         <v>5</v>
@@ -1228,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="1"/>
@@ -1248,12 +1246,12 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="4">
         <v>7</v>
@@ -1265,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="4">
         <v>7</v>
@@ -1277,7 +1275,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="1"/>
@@ -1297,12 +1295,12 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4">
         <v>8</v>
@@ -1346,13 +1344,11 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C26" s="17"/>
       <c r="D26" s="8">
         <f>SUM(D20:D25)</f>
         <v>47</v>
@@ -1403,14 +1399,14 @@
       </c>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>15</v>
+      <c r="A27" s="26" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="12">
         <v>16</v>
@@ -1454,12 +1450,12 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4">
         <v>15</v>
@@ -1471,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="4">
         <v>14</v>
@@ -1483,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" ref="L28:L31" si="7">H28-D28</f>
@@ -1503,12 +1499,12 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="4">
         <v>14</v>
@@ -1520,7 +1516,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H29" s="4">
         <v>13</v>
@@ -1532,7 +1528,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="7"/>
@@ -1552,12 +1548,12 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="4">
         <v>13</v>
@@ -1569,7 +1565,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="4">
         <v>13</v>
@@ -1581,7 +1577,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="7"/>
@@ -1601,12 +1597,12 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D31" s="4">
         <v>12</v>
@@ -1650,13 +1646,11 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C32" s="17"/>
       <c r="D32" s="8">
         <f>SUM(D27:D31)</f>
         <v>70</v>
@@ -1708,6 +1702,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L17:O18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="A20:A26"/>
@@ -1715,11 +1714,6 @@
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="H17:K17"/>
-    <mergeCell ref="L17:O18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:O32 L20:O25">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="notEqual">
@@ -1745,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A15:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1769,85 +1763,85 @@
   </cols>
   <sheetData>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="51" t="s">
+      <c r="D15" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-    </row>
-    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="38" t="s">
+      <c r="A17" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49" t="s">
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="24" t="s">
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="37"/>
       <c r="P17" s="23"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="30" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32" t="s">
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="29"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="40"/>
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="46"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1887,14 +1881,14 @@
       <c r="P19" s="23"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
-        <v>14</v>
+      <c r="A20" s="26" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="4">
         <v>9</v>
@@ -1938,12 +1932,12 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="4">
         <v>8</v>
@@ -1955,7 +1949,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="4">
         <v>7</v>
@@ -1967,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="K21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L21" s="5">
         <f t="shared" ref="L21:M32" si="1">H21-D21</f>
@@ -1987,12 +1981,12 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="42"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="4">
         <v>9</v>
@@ -2004,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
@@ -2016,7 +2010,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L22" s="5">
         <f t="shared" si="1"/>
@@ -2036,12 +2030,12 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" s="4">
         <v>10</v>
@@ -2053,7 +2047,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="4">
         <v>5</v>
@@ -2065,7 +2059,7 @@
         <v>3</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="5">
         <f t="shared" si="1"/>
@@ -2085,12 +2079,12 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="42"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" s="4">
         <v>8</v>
@@ -2102,7 +2096,7 @@
         <v>5</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="4">
         <v>7</v>
@@ -2114,7 +2108,7 @@
         <v>6</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L24" s="5">
         <f t="shared" si="1"/>
@@ -2134,12 +2128,12 @@
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" s="4">
         <v>9</v>
@@ -2183,13 +2177,11 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C26" s="17"/>
       <c r="D26" s="8">
         <f>SUM(D20:D25)</f>
         <v>53</v>
@@ -2240,14 +2232,14 @@
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
-        <v>15</v>
+      <c r="A27" s="26" t="s">
+        <v>14</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="12">
         <v>17</v>
@@ -2291,12 +2283,12 @@
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
+      <c r="A28" s="27"/>
       <c r="B28" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="4">
         <v>16</v>
@@ -2308,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H28" s="4">
         <v>14</v>
@@ -2320,7 +2312,7 @@
         <v>3</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="1"/>
@@ -2340,12 +2332,12 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="42"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="4">
         <v>15</v>
@@ -2357,7 +2349,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H29" s="4">
         <v>13</v>
@@ -2369,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="1"/>
@@ -2389,12 +2381,12 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="42"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="4">
         <v>14</v>
@@ -2406,7 +2398,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="4">
         <v>13</v>
@@ -2418,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="1"/>
@@ -2438,12 +2430,12 @@
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="4">
         <v>13</v>
@@ -2487,13 +2479,11 @@
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="43"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>13</v>
-      </c>
+      <c r="C32" s="17"/>
       <c r="D32" s="8">
         <f>SUM(D27:D31)</f>
         <v>75</v>
@@ -2545,6 +2535,9 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L17:O18"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:K18"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="A20:A26"/>
@@ -2554,9 +2547,6 @@
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:G17"/>
     <mergeCell ref="H17:K17"/>
-    <mergeCell ref="L17:O18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="L32:O32 L20:O25">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="notEqual">

</xml_diff>

<commit_message>
Implemented #7: Add assignee column. Implemented #23: Add Component column.
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -17,14 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>IssueKey</t>
   </si>
   <si>
-    <t>02 Oct 2014 11:31 +04:00</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -38,9 +35,6 @@
   </si>
   <si>
     <t>Pile description</t>
-  </si>
-  <si>
-    <t>Root issue</t>
   </si>
   <si>
     <t>Relation
@@ -82,24 +76,6 @@
     <t>CONF-36850</t>
   </si>
   <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>CONF-36883</t>
-  </si>
-  <si>
-    <t>CONF-36875</t>
-  </si>
-  <si>
-    <t>CONF-36874</t>
-  </si>
-  <si>
-    <t>CONF-36873</t>
-  </si>
-  <si>
-    <t>CONF-36866</t>
-  </si>
-  <si>
     <t>Estimation, h</t>
   </si>
   <si>
@@ -107,6 +83,27 @@
   </si>
   <si>
     <t>Remaining, h</t>
+  </si>
+  <si>
+    <t>Component(s)</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Check multi-component</t>
+  </si>
+  <si>
+    <t>JRA-42455</t>
+  </si>
+  <si>
+    <t>JRA-42416</t>
+  </si>
+  <si>
+    <t>Check assignee person</t>
+  </si>
+  <si>
+    <t>Check issue with linked issues</t>
   </si>
 </sst>
 </file>
@@ -140,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +153,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -299,10 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -314,19 +314,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -339,9 +348,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -356,15 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -694,15 +691,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:U32"/>
+  <dimension ref="A17:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
@@ -712,8 +709,8 @@
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -724,162 +721,182 @@
     <col min="20" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+    </row>
+    <row r="18" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>6</v>
-      </c>
       <c r="B18" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="U18" s="13"/>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="38"/>
       <c r="B19" s="31"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="31"/>
       <c r="F19" s="33"/>
       <c r="G19" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
       <c r="G22" s="3"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="36"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
       <c r="G23" s="3"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="36"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="3"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="37"/>
-      <c r="B26" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="36"/>
+      <c r="B26" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
       <c r="G26" s="6">
         <f>SUM(G20:G25)</f>
         <v>0</v>
@@ -892,121 +909,44 @@
         <f>SUM(I20:I25)</f>
         <v>0</v>
       </c>
-      <c r="J26" s="8" t="e">
-        <f>H26/(H26+I26)</f>
+      <c r="J26" s="7" t="e">
+        <f>F26/(F26+G26)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26" t="s">
+      <c r="K26" s="21"/>
+      <c r="L26" s="22"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="24"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="25"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="12"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="36"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="6">
-        <f>SUM(G27:G31)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="7">
-        <f>SUM(H27:H31)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="7">
-        <f>SUM(I27:I31)</f>
-        <v>0</v>
-      </c>
-      <c r="J32" s="8" t="e">
-        <f>H32/(H32+I32)</f>
-        <v>#DIV/0!</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A32"/>
+  <mergeCells count="9">
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="G18:L18"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A20:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1018,12 +958,12 @@
   <dimension ref="A15:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
@@ -1033,8 +973,8 @@
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -1046,120 +986,126 @@
   </cols>
   <sheetData>
     <row r="15" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
     </row>
     <row r="16" spans="7:15" x14ac:dyDescent="0.25">
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>6</v>
-      </c>
       <c r="B18" s="30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="13"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="31"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="31"/>
       <c r="F19" s="33"/>
       <c r="G19" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="10"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K19" s="13"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="13"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="9"/>
+      <c r="M20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="G18:L18"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented  #35: List issues with certain labels in report.
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="19965" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19965" windowHeight="13020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Do not scan 1" sheetId="1" r:id="rId1"/>
     <sheet name="Do not scan 2" sheetId="2" r:id="rId2"/>
     <sheet name="# Scan 1 - predefined issues" sheetId="3" r:id="rId3"/>
     <sheet name="# Scan 2 - root issue" sheetId="4" r:id="rId4"/>
+    <sheet name="# Scan 3 - label" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>IssueKey</t>
   </si>
@@ -104,6 +105,12 @@
   </si>
   <si>
     <t>Check issue with linked issues</t>
+  </si>
+  <si>
+    <t>Label(s)</t>
+  </si>
+  <si>
+    <t>blitz,slush</t>
   </si>
 </sst>
 </file>
@@ -293,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -324,6 +331,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,18 +361,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,12 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A17:W28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,55 +730,55 @@
   </cols>
   <sheetData>
     <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="29"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="35"/>
       <c r="W18" s="10"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
@@ -791,7 +799,7 @@
       </c>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="36" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="17"/>
@@ -809,7 +817,7 @@
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18" t="s">
         <v>16</v>
@@ -825,7 +833,7 @@
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
+      <c r="A22" s="37"/>
       <c r="B22" s="17"/>
       <c r="C22" s="18" t="s">
         <v>15</v>
@@ -841,7 +849,7 @@
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
+      <c r="A23" s="37"/>
       <c r="B23" s="17"/>
       <c r="C23" s="18" t="s">
         <v>14</v>
@@ -857,7 +865,7 @@
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
+      <c r="A24" s="37"/>
       <c r="B24" s="17"/>
       <c r="C24" s="18" t="s">
         <v>13</v>
@@ -873,7 +881,7 @@
       <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="17"/>
       <c r="C25" s="18" t="s">
         <v>12</v>
@@ -889,7 +897,7 @@
       <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="19" t="s">
         <v>2</v>
       </c>
@@ -938,6 +946,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A20:A26"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
@@ -946,7 +955,6 @@
     <mergeCell ref="G18:L18"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A20:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -958,7 +966,7 @@
   <dimension ref="A15:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="A17" sqref="A17:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,58 +1016,58 @@
       <c r="O16" s="16"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="29"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="35"/>
       <c r="M18" s="10"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="33"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1110,4 +1118,125 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A17:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="35"/>
+      <c r="M18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="39" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="L20" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:L18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed #44: Application crashes if issue is not found!
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="19965" windowHeight="12960" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="19965" windowHeight="12960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Do not scan 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
   <si>
     <t>IssueKey</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Gadgets</t>
+  </si>
+  <si>
+    <t>Missing issue</t>
+  </si>
+  <si>
+    <t>JRA-99999</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -474,6 +480,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,10 +808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,37 +1074,55 @@
       <c r="K13" s="22"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="E5:L5"/>
@@ -1286,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented #30: Release 0.2.8.
</commit_message>
<xml_diff>
--- a/default.xlsx
+++ b/default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="19965" windowHeight="12960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="19965" windowHeight="12960" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Do not scan 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>IssueKey</t>
   </si>
@@ -453,6 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -480,7 +481,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="I2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,7 +824,7 @@
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -839,20 +839,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -869,7 +869,9 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="J2" s="12" t="s">
         <v>24</v>
       </c>
@@ -893,34 +895,34 @@
       <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="30"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1080,7 @@
       <c r="A14" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="24" t="s">
         <v>36</v>
       </c>
       <c r="C14" s="9"/>
@@ -1144,7 +1146,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="I2" sqref="I2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1159,7 @@
     <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1172,20 +1174,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1202,7 +1204,9 @@
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="I2" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="J2" s="12" t="s">
         <v>24</v>
       </c>
@@ -1228,34 +1232,34 @@
       <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="30"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1311,7 +1315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -1333,20 +1337,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -1395,34 +1399,34 @@
       <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="30"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>